<commit_message>
Basic Landing Page 0
</commit_message>
<xml_diff>
--- a/backend/data/synthetic/gstr1.xlsx
+++ b/backend/data/synthetic/gstr1.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -518,7 +518,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -548,7 +548,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -578,7 +578,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -608,7 +608,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -638,7 +638,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -668,7 +668,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -698,7 +698,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -728,7 +728,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -758,7 +758,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -788,7 +788,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -818,7 +818,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -848,7 +848,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -878,7 +878,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -908,7 +908,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -938,7 +938,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -968,7 +968,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -998,7 +998,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -1808,7 +1808,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -1958,7 +1958,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2108,7 +2108,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F60" t="n">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F61" t="n">
@@ -2288,7 +2288,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F63" t="n">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F64" t="n">
@@ -2378,7 +2378,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F66" t="n">
@@ -2438,7 +2438,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F67" t="n">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F68" t="n">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F69" t="n">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F71" t="n">
@@ -2588,7 +2588,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F72" t="n">
@@ -2618,7 +2618,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F73" t="n">
@@ -2648,7 +2648,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F74" t="n">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F76" t="n">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F77" t="n">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F78" t="n">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F79" t="n">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F80" t="n">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F81" t="n">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F82" t="n">
@@ -2918,7 +2918,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F83" t="n">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F84" t="n">
@@ -2978,7 +2978,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F85" t="n">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F86" t="n">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F87" t="n">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F88" t="n">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F89" t="n">
@@ -3128,7 +3128,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F90" t="n">
@@ -3158,7 +3158,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F91" t="n">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F92" t="n">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F93" t="n">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F94" t="n">
@@ -3278,7 +3278,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F95" t="n">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F96" t="n">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F97" t="n">
@@ -3368,7 +3368,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F98" t="n">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F99" t="n">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F100" t="n">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F101" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F102" t="n">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F103" t="n">
@@ -3548,7 +3548,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F104" t="n">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F105" t="n">
@@ -3608,7 +3608,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F106" t="n">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F107" t="n">
@@ -3668,7 +3668,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F108" t="n">
@@ -3698,7 +3698,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F109" t="n">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F110" t="n">
@@ -3758,7 +3758,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F111" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F112" t="n">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F113" t="n">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F114" t="n">
@@ -3878,7 +3878,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F115" t="n">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F116" t="n">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F117" t="n">
@@ -3968,7 +3968,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F118" t="n">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F119" t="n">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F120" t="n">
@@ -4058,7 +4058,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F121" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F122" t="n">
@@ -4118,7 +4118,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F123" t="n">
@@ -4148,7 +4148,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F124" t="n">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F125" t="n">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F126" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F127" t="n">
@@ -4268,7 +4268,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F128" t="n">
@@ -4298,7 +4298,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F129" t="n">
@@ -4328,7 +4328,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F130" t="n">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F131" t="n">
@@ -4388,7 +4388,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F132" t="n">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F133" t="n">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F134" t="n">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F135" t="n">
@@ -4508,7 +4508,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F136" t="n">
@@ -4538,7 +4538,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F137" t="n">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F138" t="n">
@@ -4598,7 +4598,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F139" t="n">
@@ -4628,7 +4628,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F140" t="n">
@@ -4658,7 +4658,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F141" t="n">
@@ -4688,7 +4688,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F142" t="n">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F143" t="n">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F144" t="n">
@@ -4778,7 +4778,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F145" t="n">
@@ -4808,7 +4808,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F146" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F147" t="n">
@@ -4868,7 +4868,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F148" t="n">
@@ -4898,7 +4898,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F149" t="n">
@@ -4928,7 +4928,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F150" t="n">
@@ -4958,7 +4958,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F151" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F152" t="n">
@@ -5018,7 +5018,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F153" t="n">
@@ -5048,7 +5048,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F154" t="n">
@@ -5078,7 +5078,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F155" t="n">
@@ -5108,7 +5108,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F156" t="n">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F157" t="n">
@@ -5168,7 +5168,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F158" t="n">
@@ -5198,7 +5198,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F159" t="n">
@@ -5228,7 +5228,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F160" t="n">
@@ -5258,7 +5258,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F161" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F162" t="n">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F163" t="n">
@@ -5348,7 +5348,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F164" t="n">
@@ -5378,7 +5378,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F165" t="n">
@@ -5408,7 +5408,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F166" t="n">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F167" t="n">
@@ -5468,7 +5468,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F168" t="n">
@@ -5498,7 +5498,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F169" t="n">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F170" t="n">
@@ -5558,7 +5558,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F171" t="n">
@@ -5588,7 +5588,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F172" t="n">
@@ -5618,7 +5618,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F173" t="n">
@@ -5648,7 +5648,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F174" t="n">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F175" t="n">
@@ -5708,7 +5708,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F176" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F177" t="n">
@@ -5768,7 +5768,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F178" t="n">
@@ -5798,7 +5798,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F179" t="n">
@@ -5828,7 +5828,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F180" t="n">
@@ -5858,7 +5858,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F181" t="n">
@@ -5888,7 +5888,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F182" t="n">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F183" t="n">
@@ -5948,7 +5948,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F184" t="n">
@@ -5978,7 +5978,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F185" t="n">
@@ -6008,7 +6008,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F186" t="n">
@@ -6038,7 +6038,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F187" t="n">
@@ -6068,7 +6068,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F188" t="n">
@@ -6098,7 +6098,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F189" t="n">
@@ -6128,7 +6128,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F190" t="n">
@@ -6158,7 +6158,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F191" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F192" t="n">
@@ -6218,7 +6218,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F193" t="n">
@@ -6248,7 +6248,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F194" t="n">
@@ -6278,7 +6278,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F195" t="n">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F196" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F197" t="n">
@@ -6368,7 +6368,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F198" t="n">
@@ -6398,7 +6398,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F199" t="n">
@@ -6428,7 +6428,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F200" t="n">
@@ -6458,7 +6458,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F201" t="n">
@@ -6488,7 +6488,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F202" t="n">
@@ -6518,7 +6518,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F203" t="n">
@@ -6548,7 +6548,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F204" t="n">
@@ -6578,7 +6578,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F205" t="n">
@@ -6608,7 +6608,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F206" t="n">
@@ -6638,7 +6638,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F207" t="n">
@@ -6668,7 +6668,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F208" t="n">
@@ -6698,7 +6698,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F209" t="n">
@@ -6728,7 +6728,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F210" t="n">
@@ -6758,7 +6758,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F211" t="n">
@@ -6788,7 +6788,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F212" t="n">
@@ -6818,7 +6818,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F213" t="n">
@@ -6848,7 +6848,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F214" t="n">
@@ -6878,7 +6878,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F215" t="n">
@@ -6908,7 +6908,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F216" t="n">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F217" t="n">
@@ -6968,7 +6968,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F218" t="n">
@@ -6998,7 +6998,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F219" t="n">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F220" t="n">
@@ -7058,7 +7058,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F221" t="n">
@@ -7088,7 +7088,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F222" t="n">
@@ -7118,7 +7118,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F223" t="n">
@@ -7148,7 +7148,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F224" t="n">
@@ -7178,7 +7178,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F225" t="n">
@@ -7208,7 +7208,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F226" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F227" t="n">
@@ -7268,7 +7268,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F228" t="n">
@@ -7298,7 +7298,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F229" t="n">
@@ -7328,7 +7328,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F230" t="n">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F231" t="n">
@@ -7388,7 +7388,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F232" t="n">
@@ -7418,7 +7418,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F233" t="n">
@@ -7448,7 +7448,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F234" t="n">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F235" t="n">
@@ -7508,7 +7508,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F236" t="n">
@@ -7538,7 +7538,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F237" t="n">
@@ -7568,7 +7568,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F238" t="n">
@@ -7598,7 +7598,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F239" t="n">
@@ -7628,7 +7628,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F240" t="n">
@@ -7658,7 +7658,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F241" t="n">
@@ -7688,7 +7688,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F242" t="n">
@@ -7718,7 +7718,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F243" t="n">
@@ -7748,7 +7748,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F244" t="n">
@@ -7778,7 +7778,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F245" t="n">
@@ -7808,7 +7808,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F246" t="n">
@@ -7838,7 +7838,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F247" t="n">
@@ -7868,7 +7868,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F248" t="n">
@@ -7898,7 +7898,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F249" t="n">
@@ -7928,7 +7928,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F250" t="n">
@@ -7958,7 +7958,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F251" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F252" t="n">
@@ -8018,7 +8018,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F253" t="n">
@@ -8048,7 +8048,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F254" t="n">
@@ -8078,7 +8078,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F255" t="n">
@@ -8108,7 +8108,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F256" t="n">
@@ -8138,7 +8138,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F257" t="n">
@@ -8168,7 +8168,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F258" t="n">
@@ -8198,7 +8198,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F259" t="n">
@@ -8228,7 +8228,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F260" t="n">
@@ -8258,7 +8258,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F261" t="n">
@@ -8288,7 +8288,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F262" t="n">
@@ -8318,7 +8318,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F263" t="n">
@@ -8348,7 +8348,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F264" t="n">
@@ -8378,7 +8378,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F265" t="n">
@@ -8408,7 +8408,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F266" t="n">
@@ -8438,7 +8438,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F267" t="n">
@@ -8468,7 +8468,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F268" t="n">
@@ -8498,7 +8498,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F269" t="n">
@@ -8528,7 +8528,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F270" t="n">
@@ -8558,7 +8558,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F271" t="n">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F272" t="n">
@@ -8618,7 +8618,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F273" t="n">
@@ -8648,7 +8648,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F274" t="n">
@@ -8678,7 +8678,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F275" t="n">
@@ -8708,7 +8708,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F276" t="n">
@@ -8738,7 +8738,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F277" t="n">
@@ -8768,7 +8768,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F278" t="n">
@@ -8798,7 +8798,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F279" t="n">
@@ -8828,7 +8828,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F280" t="n">
@@ -8858,7 +8858,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F281" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F282" t="n">
@@ -8918,7 +8918,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F283" t="n">
@@ -8948,7 +8948,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F284" t="n">
@@ -8978,7 +8978,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F285" t="n">
@@ -9008,7 +9008,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F286" t="n">
@@ -9038,7 +9038,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F287" t="n">
@@ -9068,7 +9068,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F288" t="n">
@@ -9098,7 +9098,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F289" t="n">
@@ -9128,7 +9128,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F290" t="n">
@@ -9158,7 +9158,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F291" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F292" t="n">
@@ -9218,7 +9218,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F293" t="n">
@@ -9248,7 +9248,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F294" t="n">
@@ -9278,7 +9278,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F295" t="n">
@@ -9308,7 +9308,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F296" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F297" t="n">
@@ -9368,7 +9368,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F298" t="n">
@@ -9398,7 +9398,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F299" t="n">
@@ -9428,7 +9428,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F300" t="n">
@@ -9458,7 +9458,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Filed</t>
+          <t>FILED</t>
         </is>
       </c>
       <c r="F301" t="n">

</xml_diff>